<commit_message>
Add new analyte class Lipid + metabolite + protein
Closes #138
</commit_message>
<xml_diff>
--- a/enhanced-srs/latest/enhanced-srs.xlsx
+++ b/enhanced-srs/latest/enhanced-srs.xlsx
@@ -1,135 +1,267 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josefhardi/Documents/Code/dataset-metadata-spreadsheet/enhanced-srs/latest/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ED11F8-620F-7C40-948F-CA3D6B68B7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="21680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Enhanced SRS" r:id="rId3" sheetId="1"/>
-    <sheet name="dataset_type" r:id="rId4" sheetId="2"/>
-    <sheet name="analyte_class" r:id="rId5" sheetId="3"/>
-    <sheet name="is_targeted" r:id="rId6" sheetId="4"/>
-    <sheet name="acquisition_instrument_vendor" r:id="rId7" sheetId="5"/>
-    <sheet name="acquisition_instrument_model" r:id="rId8" sheetId="6"/>
-    <sheet name="source_storage_duration_unit" r:id="rId9" sheetId="7"/>
-    <sheet name="time_since_acquisition_instrume" r:id="rId10" sheetId="8"/>
-    <sheet name="is_image_preprocessing_required" r:id="rId11" sheetId="9"/>
-    <sheet name="tile_configuration" r:id="rId12" sheetId="10"/>
-    <sheet name="scan_direction" r:id="rId13" sheetId="11"/>
-    <sheet name=".metadata" r:id="rId14" sheetId="12"/>
+    <sheet name="Enhanced SRS" sheetId="1" r:id="rId1"/>
+    <sheet name="dataset_type" sheetId="2" r:id="rId2"/>
+    <sheet name="analyte_class" sheetId="3" r:id="rId3"/>
+    <sheet name="is_targeted" sheetId="4" r:id="rId4"/>
+    <sheet name="acquisition_instrument_vendor" sheetId="5" r:id="rId5"/>
+    <sheet name="acquisition_instrument_model" sheetId="6" r:id="rId6"/>
+    <sheet name="source_storage_duration_unit" sheetId="7" r:id="rId7"/>
+    <sheet name="time_since_acquisition_instrume" sheetId="8" r:id="rId8"/>
+    <sheet name="is_image_preprocessing_required" sheetId="9" r:id="rId9"/>
+    <sheet name="tile_configuration" sheetId="10" r:id="rId10"/>
+    <sheet name="scan_direction" sheetId="11" r:id="rId11"/>
+    <sheet name=".metadata" sheetId="12" r:id="rId12"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author/>
     <author>CEDAR Metadata Validator</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="1">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
 block, section, or suspension) used to perform the assay. For instance, in an
 RNAseq assay, the parent sample would be the suspension, while in imaging
 assays, it would be the tissue section. If the assay is derived from multiple
 parent samples, this field should contain a comma-separated list of identifiers.
 Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
+        </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="1">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
-        <t>A locally assigned identifier provided by the data provider for the dataset. It
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>A locally assigned identifier provided by the data provider for the dataset. It
 is used to reference an external metadata record that may be maintained
 independently, enabling traceability and supporting provenance tracking.
 Example: Visium_9OLC_A4_S1</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <t>(Required) The DOI for the protocols.io page that details the assay or the
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The DOI for the protocols.io page that details the assay or the
 procedures used for sample procurement and preparation. For example, in the case
 of an imaging assay, the protocol may start with tissue section staining and end
 with the generation of an OME-TIFF file. The documented protocol should also
 include any image processing steps involved in producing the final OME-TIFF.
 Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
-        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
-        <t>(Required) The analyte class which is the target molecule that the assay is
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The analyte class which is the target molecule that the assay is
 measuring. Example: DNA</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="1">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
-        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
 for detection or measurement by the assay. Example: Yes</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="1">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
-        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The company that manufactures or supplies the acquisition instrument.
 An acquisition instrument is a device equipped with signal detection hardware
 and signal processing software. It captures signals produced by assays, such as
 variations in light intensity or color, or signals corresponding to molecular
 mass. If the instrument was custom-built or developed internally, enter
 "In-House". Example: Illumina</t>
+        </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="1">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
-        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The specific model of the acquisition instrument, as manufacturers
 often offer various versions with differing features or sensitivities. These
 differences may be relevant to the processing or interpretation of the data. If
 the instrument was custom-built or developed internally, enter "In-House". If
 the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="1">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
-        <t>(Required) The length of time the sample was stored prior to processing it. For
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The length of time the sample was stored prior to processing it. For
 assays performed on tissue sections, this refers to how long the tissue section
 (e.g., slide) was stored before the assay began (e.g., imaging). For assays
 performed on suspensions, such as sequencing, it refers to how long the
 suspension was stored before library construction started. Example: 12</t>
+        </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
-        <t>(Required) The unit of measurement used to specify the source storage duration
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The unit of measurement used to specify the source storage duration
 value. Example: hour</t>
+        </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="1">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
-        <t>The length of time since the acquisition instrument was last serviced or
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The length of time since the acquisition instrument was last serviced or
 calibrated. This provides a metric for assessing drift in data capture. Example:
 10</t>
+        </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
-        <t>The unit of measurement used to specify the time since acquisition instrument
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The unit of measurement used to specify the time since acquisition instrument
 calibration value. Example: month</t>
+        </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
-        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The name of the file containing the ORCID IDs for all contributors to
 this dataset. Example: ./contributors.csv</t>
+        </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
-        <t>(Required) The top-level directory containing the raw and/or processed data. For
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The top-level directory containing the raw and/or processed data. For
 a single dataset upload, this might be represented as ".", whereas for a data
 upload containing multiple datasets, this would be the directory name for the
 respective dataset. For example, if the data is within a directory named
@@ -137,60 +269,133 @@
 multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
 "Pass2" is the subdirectory where the single dataset's data is stored. This is
 an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
+        </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
-        <t>Indicates whether image preprocessing is necessary based on the type of
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Indicates whether image preprocessing is necessary based on the type of
 acquisition instrument used, such as a microscope or slide scanner. This may
 involve steps like fusing image tiles to assemble the complete image. Example:
 Yes</t>
+        </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
-        <t>The unique identifier assigned to each slide, enabling users to determine which
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The unique identifier assigned to each slide, enabling users to determine which
 tissue sections were processed together on the same slide. It is recommended
 that data providers prefix the ID with the center name to prevent overlapping
 values across different centers. Example: VAN0071-PA-1-1_AF</t>
+        </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
-        <t>The configuration of tiles used for stitching in the assay process. If no tile
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The configuration of tiles used for stitching in the assay process. If no tile
 configuration is applicable, enter "Not applicable". Example: Row-by-row</t>
+        </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
-        <t>The direction of imaging, which is necessary for the stitching process. Example:
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The direction of imaging, which is necessary for the stitching process. Example:
 Left-and-down</t>
+        </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
-        <t>The number of columns used in the stitching process of a tiled image, often
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of columns used in the stitching process of a tiled image, often
 referred to as the grid size in the x-dimension. Example: 5</t>
+        </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
-        <t>The total number of raw tiled images captured, which are intended to be stitched
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The total number of raw tiled images captured, which are intended to be stitched
 together. Example: 75</t>
+        </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
-        <t>The intended percentage of overlap between tiled images. This value serves as
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The intended percentage of overlap between tiled images. This value serves as
 the set point, although slight variations may occur during image acquisition due
 to stage registration. Example: 5</t>
+        </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
-        <t>(Required) The unique string identifier for the metadata specification version,
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>(Required) The unique string identifier for the metadata specification version,
 which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -198,7 +403,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="428">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -500,6 +705,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
   </si>
   <si>
+    <t>Raman Imaging</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000475</t>
+  </si>
+  <si>
     <t>RNAseq (with probes)</t>
   </si>
   <si>
@@ -512,6 +723,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
+    <t>STARmap</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000476</t>
+  </si>
+  <si>
     <t>MPLEx</t>
   </si>
   <si>
@@ -725,6 +942,12 @@
     <t>https://identifiers.org/RRID:SCR_023605</t>
   </si>
   <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024589</t>
+  </si>
+  <si>
     <t>In-House</t>
   </si>
   <si>
@@ -785,6 +1008,12 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Revvity</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027779</t>
+  </si>
+  <si>
     <t>Cytek Biosciences</t>
   </si>
   <si>
@@ -914,6 +1143,18 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>DMi8</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026672</t>
+  </si>
+  <si>
+    <t>Opera Phenix Plus HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027780</t>
+  </si>
+  <si>
     <t>timsTOF Pro 2</t>
   </si>
   <si>
@@ -956,6 +1197,12 @@
     <t>https://identifiers.org/RRID:SCR_027101</t>
   </si>
   <si>
+    <t>Orbitrap Fusion Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020559</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1082,6 +1329,18 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Opera Phenix HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027817</t>
+  </si>
+  <si>
+    <t>Zeiss LightSheet Z.1</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020919</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1223,6 +1482,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>SYNAPT G2-Si</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027782</t>
+  </si>
+  <si>
     <t>Biomark HD</t>
   </si>
   <si>
@@ -1409,45 +1674,48 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-11-20T09:37:19-08:00</t>
+    <t>2026-01-14T11:46:17-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
   </si>
   <si>
     <t>https://repo.metadatacenter.org/templates/609c3adb-e65d-4124-bb1b-dd937f231850</t>
+  </si>
+  <si>
+    <t>Lipid + metabolite + protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000478</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode=""/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1465,1948 +1733,2370 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="2" width="14.39453125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="3" width="5.46875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="4" width="20.234375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="5" width="10.59765625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="10.9296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="9.40234375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="8" width="24.5546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="9" width="24.0390625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="10" width="24.63671875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="11" width="23.63671875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="12" width="41.1015625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="13" width="40.1015625" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="14" width="14.5859375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" style="15" width="8.46484375" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" style="16" width="26.5625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" style="17" width="6.7421875" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="14.3671875" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="11.953125" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="17.0234375" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" style="21" width="14.875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" style="22" width="26.59765625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" style="23" width="16.91796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
-        <v>106</v>
-      </c>
-      <c r="F1" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="G1" t="s" s="1">
-        <v>144</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>205</v>
-      </c>
-      <c r="I1" t="s" s="1">
-        <v>357</v>
-      </c>
-      <c r="J1" t="s" s="1">
-        <v>358</v>
-      </c>
-      <c r="K1" t="s" s="1">
-        <v>369</v>
-      </c>
-      <c r="L1" t="s" s="1">
-        <v>370</v>
-      </c>
-      <c r="M1" t="s" s="1">
-        <v>371</v>
-      </c>
-      <c r="N1" t="s" s="1">
-        <v>372</v>
-      </c>
-      <c r="O1" t="s" s="1">
-        <v>373</v>
-      </c>
-      <c r="P1" t="s" s="1">
-        <v>374</v>
-      </c>
-      <c r="Q1" t="s" s="1">
-        <v>375</v>
-      </c>
-      <c r="R1" t="s" s="1">
-        <v>384</v>
-      </c>
-      <c r="S1" t="s" s="1">
+      <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="T1" t="s" s="1">
+      <c r="P1" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="U1" t="s" s="1">
+      <c r="Q1" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="V1" t="s" s="1">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="D2" t="s" s="5">
+      <c r="R1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="V2" t="s" s="23">
-        <v>397</v>
+      <c r="V2" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
-    <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$51</formula1>
+  <dataValidations count="2">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" error="Value should be greater than 0" sqref="I2:I1001 U2:U1001 K2:K1001" xr:uid="{00000000-0002-0000-0000-000005000000}">
+      <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$17</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'is_targeted'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
-      <formula1>0</formula1>
-      <formula2/>
-    </dataValidation>
-    <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'source_storage_duration_unit'!$A$1:$A$5</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
-      <formula1>0</formula1>
-      <formula2/>
-    </dataValidation>
-    <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'is_image_preprocessing_required'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'tile_configuration'!$A$1:$A$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'scan_direction'!$A$1:$A$5</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 1" showErrorMessage="true">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" error="Value should be greater than 1" sqref="S2:T1001" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>1</formula1>
-      <formula2/>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 1" showErrorMessage="true">
-      <formula1>1</formula1>
-      <formula2/>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
-      <formula1>0</formula1>
-      <formula2/>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>dataset_type!$A$1:$A$53</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000001000000}">
+          <x14:formula1>
+            <xm:f>analyte_class!$A$1:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000002000000}">
+          <x14:formula1>
+            <xm:f>is_targeted!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000003000000}">
+          <x14:formula1>
+            <xm:f>acquisition_instrument_vendor!$A$1:$A$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000004000000}">
+          <x14:formula1>
+            <xm:f>acquisition_instrument_model!$A$1:$A$83</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000006000000}">
+          <x14:formula1>
+            <xm:f>source_storage_duration_unit!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000008000000}">
+          <x14:formula1>
+            <xm:f>time_since_acquisition_instrume!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000009000000}">
+          <x14:formula1>
+            <xm:f>is_image_preprocessing_required!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+          <x14:formula1>
+            <xm:f>tile_configuration!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+          <x14:formula1>
+            <xm:f>scan_direction!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R1001</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>214</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>376</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>378</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>380</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>382</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>383</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B5" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>385</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>387</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>214</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>389</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>391</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>392</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B5" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="70.0546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>398</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>400</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>402</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>399</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>403</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>405</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D2" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="B24" t="s" s="0">
+      <c r="B24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B25" t="s" s="0">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>54</v>
       </c>
-      <c r="B26" t="s" s="0">
+      <c r="B26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s" s="0">
+      <c r="B27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-      <c r="B28" t="s" s="0">
+      <c r="B28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>60</v>
       </c>
-      <c r="B29" t="s" s="0">
+      <c r="B29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>62</v>
       </c>
-      <c r="B30" t="s" s="0">
+      <c r="B30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>64</v>
       </c>
-      <c r="B31" t="s" s="0">
+      <c r="B31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>66</v>
       </c>
-      <c r="B32" t="s" s="0">
+      <c r="B32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>68</v>
       </c>
-      <c r="B33" t="s" s="0">
+      <c r="B33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>70</v>
       </c>
-      <c r="B34" t="s" s="0">
+      <c r="B34" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>72</v>
       </c>
-      <c r="B35" t="s" s="0">
+      <c r="B35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>74</v>
       </c>
-      <c r="B36" t="s" s="0">
+      <c r="B36" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>76</v>
       </c>
-      <c r="B37" t="s" s="0">
+      <c r="B37" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>78</v>
       </c>
-      <c r="B38" t="s" s="0">
+      <c r="B38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>80</v>
       </c>
-      <c r="B39" t="s" s="0">
+      <c r="B39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s" s="0">
+      <c r="B40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>84</v>
       </c>
-      <c r="B41" t="s" s="0">
+      <c r="B41" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>86</v>
       </c>
-      <c r="B42" t="s" s="0">
+      <c r="B42" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="s" s="0">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>88</v>
       </c>
-      <c r="B43" t="s" s="0">
+      <c r="B43" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="s" s="0">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>90</v>
       </c>
-      <c r="B44" t="s" s="0">
+      <c r="B44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="s" s="0">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>92</v>
       </c>
-      <c r="B45" t="s" s="0">
+      <c r="B45" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>94</v>
       </c>
-      <c r="B46" t="s" s="0">
+      <c r="B46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>96</v>
       </c>
-      <c r="B47" t="s" s="0">
+      <c r="B47" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B48" t="s" s="0">
+      <c r="B48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="s" s="0">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>100</v>
       </c>
-      <c r="B49" t="s" s="0">
+      <c r="B49" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="s" s="0">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>102</v>
       </c>
-      <c r="B50" t="s" s="0">
+      <c r="B50" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="s" s="0">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>104</v>
       </c>
-      <c r="B51" t="s" s="0">
+      <c r="B51" t="s">
         <v>105</v>
       </c>
     </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>111</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>113</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>115</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>117</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>121</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>123</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>125</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>426</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>127</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>129</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>131</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>133</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>135</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>137</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>139</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B16" t="s">
         <v>140</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" location="HRAVS_0000478" xr:uid="{11DD7DDE-6105-2E43-BFD8-0A37D600F901}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>143</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>147</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>149</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>151</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>153</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>155</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>157</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>159</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>161</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>163</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>165</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>167</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>169</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>171</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>173</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>175</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>177</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>179</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B16" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>181</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B17" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>183</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B18" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>185</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>187</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B20" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>189</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B21" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>191</v>
       </c>
-      <c r="B24" t="s" s="0">
+      <c r="B22" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>193</v>
       </c>
-      <c r="B25" t="s" s="0">
+      <c r="B23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>195</v>
       </c>
-      <c r="B26" t="s" s="0">
+      <c r="B24" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>197</v>
       </c>
-      <c r="B27" t="s" s="0">
+      <c r="B25" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>199</v>
       </c>
-      <c r="B28" t="s" s="0">
+      <c r="B26" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>201</v>
       </c>
-      <c r="B29" t="s" s="0">
+      <c r="B27" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>203</v>
       </c>
-      <c r="B30" t="s" s="0">
+      <c r="B28" t="s">
         <v>204</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>205</v>
+      </c>
+      <c r="B29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B32" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>206</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>208</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>210</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>212</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>214</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>216</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>218</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>220</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>222</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B5" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>224</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>226</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>228</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B8" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>230</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>232</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B10" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>234</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B11" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>236</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B12" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>238</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B13" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>240</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B14" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>242</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B15" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>244</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B16" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>246</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>248</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B18" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>250</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B19" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>252</v>
       </c>
-      <c r="B24" t="s" s="0">
+      <c r="B20" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>254</v>
       </c>
-      <c r="B25" t="s" s="0">
+      <c r="B21" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>256</v>
       </c>
-      <c r="B26" t="s" s="0">
+      <c r="B22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>258</v>
       </c>
-      <c r="B27" t="s" s="0">
+      <c r="B23" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>260</v>
       </c>
-      <c r="B28" t="s" s="0">
+      <c r="B24" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>262</v>
       </c>
-      <c r="B29" t="s" s="0">
+      <c r="B25" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>264</v>
       </c>
-      <c r="B30" t="s" s="0">
+      <c r="B26" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>266</v>
       </c>
-      <c r="B31" t="s" s="0">
+      <c r="B27" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>268</v>
       </c>
-      <c r="B32" t="s" s="0">
+      <c r="B28" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>270</v>
       </c>
-      <c r="B33" t="s" s="0">
+      <c r="B29" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>272</v>
       </c>
-      <c r="B34" t="s" s="0">
+      <c r="B30" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>274</v>
       </c>
-      <c r="B35" t="s" s="0">
+      <c r="B31" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>276</v>
       </c>
-      <c r="B36" t="s" s="0">
+      <c r="B32" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>278</v>
       </c>
-      <c r="B37" t="s" s="0">
+      <c r="B33" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>280</v>
       </c>
-      <c r="B38" t="s" s="0">
+      <c r="B34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>282</v>
       </c>
-      <c r="B39" t="s" s="0">
+      <c r="B35" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>284</v>
       </c>
-      <c r="B40" t="s" s="0">
+      <c r="B36" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>286</v>
       </c>
-      <c r="B41" t="s" s="0">
+      <c r="B37" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>288</v>
       </c>
-      <c r="B42" t="s" s="0">
+      <c r="B38" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="s" s="0">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>290</v>
       </c>
-      <c r="B43" t="s" s="0">
+      <c r="B39" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="s" s="0">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>292</v>
       </c>
-      <c r="B44" t="s" s="0">
+      <c r="B40" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="s" s="0">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>294</v>
       </c>
-      <c r="B45" t="s" s="0">
+      <c r="B41" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>296</v>
       </c>
-      <c r="B46" t="s" s="0">
+      <c r="B42" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>298</v>
       </c>
-      <c r="B47" t="s" s="0">
+      <c r="B43" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>300</v>
       </c>
-      <c r="B48" t="s" s="0">
+      <c r="B44" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="s" s="0">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>302</v>
       </c>
-      <c r="B49" t="s" s="0">
+      <c r="B45" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="s" s="0">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>304</v>
       </c>
-      <c r="B50" t="s" s="0">
+      <c r="B46" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="s" s="0">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>306</v>
       </c>
-      <c r="B51" t="s" s="0">
+      <c r="B47" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="s" s="0">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>308</v>
       </c>
-      <c r="B52" t="s" s="0">
+      <c r="B48" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="s" s="0">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>310</v>
       </c>
-      <c r="B53" t="s" s="0">
+      <c r="B49" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="s" s="0">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>312</v>
       </c>
-      <c r="B54" t="s" s="0">
+      <c r="B50" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="s" s="0">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>314</v>
       </c>
-      <c r="B55" t="s" s="0">
+      <c r="B51" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s" s="0">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>316</v>
       </c>
-      <c r="B56" t="s" s="0">
+      <c r="B52" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s" s="0">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>318</v>
       </c>
-      <c r="B57" t="s" s="0">
+      <c r="B53" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="s" s="0">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>320</v>
       </c>
-      <c r="B58" t="s" s="0">
+      <c r="B54" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="0">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>322</v>
       </c>
-      <c r="B59" t="s" s="0">
+      <c r="B55" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="s" s="0">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>324</v>
+      </c>
+      <c r="B56" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>326</v>
+      </c>
+      <c r="B57" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>328</v>
+      </c>
+      <c r="B58" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>330</v>
+      </c>
+      <c r="B59" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>332</v>
+      </c>
+      <c r="B60" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>334</v>
+      </c>
+      <c r="B61" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>336</v>
+      </c>
+      <c r="B62" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>338</v>
+      </c>
+      <c r="B63" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>340</v>
+      </c>
+      <c r="B64" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>70</v>
       </c>
-      <c r="B60" t="s" s="0">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="0">
-        <v>325</v>
-      </c>
-      <c r="B61" t="s" s="0">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="0">
-        <v>327</v>
-      </c>
-      <c r="B62" t="s" s="0">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="0">
-        <v>329</v>
-      </c>
-      <c r="B63" t="s" s="0">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="0">
-        <v>175</v>
-      </c>
-      <c r="B64" t="s" s="0">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="0">
-        <v>331</v>
-      </c>
-      <c r="B65" t="s" s="0">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="0">
-        <v>333</v>
-      </c>
-      <c r="B66" t="s" s="0">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B67" t="s" s="0">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="0">
-        <v>337</v>
-      </c>
-      <c r="B68" t="s" s="0">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="0">
-        <v>339</v>
-      </c>
-      <c r="B69" t="s" s="0">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="0">
-        <v>341</v>
-      </c>
-      <c r="B70" t="s" s="0">
+      <c r="B65" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="s" s="0">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>343</v>
       </c>
-      <c r="B71" t="s" s="0">
+      <c r="B66" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="s" s="0">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>345</v>
       </c>
-      <c r="B72" t="s" s="0">
+      <c r="B67" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="s" s="0">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>347</v>
       </c>
-      <c r="B73" t="s" s="0">
+      <c r="B68" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="s" s="0">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>349</v>
       </c>
-      <c r="B74" t="s" s="0">
+      <c r="B70" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="s" s="0">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>351</v>
       </c>
-      <c r="B75" t="s" s="0">
+      <c r="B71" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="s" s="0">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>353</v>
       </c>
-      <c r="B76" t="s" s="0">
+      <c r="B72" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="s" s="0">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>355</v>
       </c>
-      <c r="B77" t="s" s="0">
+      <c r="B73" t="s">
         <v>356</v>
       </c>
     </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>357</v>
+      </c>
+      <c r="B74" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>359</v>
+      </c>
+      <c r="B75" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>361</v>
+      </c>
+      <c r="B76" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>363</v>
+      </c>
+      <c r="B77" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>365</v>
+      </c>
+      <c r="B78" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>367</v>
+      </c>
+      <c r="B79" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>369</v>
+      </c>
+      <c r="B80" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>371</v>
+      </c>
+      <c r="B81" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>373</v>
+      </c>
+      <c r="B82" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>375</v>
+      </c>
+      <c r="B83" t="s">
+        <v>376</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>359</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>361</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>363</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>365</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>367</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>368</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B4" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B5" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>361</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>363</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>365</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>366</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>143</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>